<commit_message>
working on Course offering
</commit_message>
<xml_diff>
--- a/Templates/Allocation and Offering Tester.xlsx
+++ b/Templates/Allocation and Offering Tester.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" tabRatio="756" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" tabRatio="756" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="BSSE-1 (Fall-2021 Batch)" sheetId="14" r:id="rId1"/>
-    <sheet name="BSSE-3 (Fall-2020 Batch)" sheetId="11" r:id="rId2"/>
+    <sheet name="BCSE-1 (Fall-2021 Batch)" sheetId="14" r:id="rId1"/>
+    <sheet name="BCSE-3 (Fall-2020 Batch)" sheetId="11" r:id="rId2"/>
     <sheet name="BCSE-5 (Fall-2019 Batch)" sheetId="12" r:id="rId3"/>
     <sheet name="BCSE-7 (Fall-2018 Batch)" sheetId="13" r:id="rId4"/>
     <sheet name="Course Allocation BSIET" sheetId="10" state="hidden" r:id="rId5"/>
@@ -192,9 +192,6 @@
     <t>SEN 432</t>
   </si>
   <si>
-    <t>BSSE-3 (Fall-2020 Batch)</t>
-  </si>
-  <si>
     <t>BCSE-5 (Fall-2019 Batch)</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
   </si>
   <si>
     <t>Applied Physics</t>
-  </si>
-  <si>
-    <t>BSSE-1 (Fall-2021 Batch)</t>
   </si>
   <si>
     <t>Data Structures &amp; Algorithms</t>
@@ -608,6 +602,12 @@
   </si>
   <si>
     <t>Section C</t>
+  </si>
+  <si>
+    <t>BCSE-1 (Fall-2021 Batch)</t>
+  </si>
+  <si>
+    <t>BCSE-3 (Fall-2020 Batch)</t>
   </si>
 </sst>
 </file>
@@ -1981,79 +1981,184 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2074,160 +2179,55 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3939,7 +3939,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3950,75 +3950,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="165" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="167"/>
+      <c r="A1" s="150" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="152"/>
     </row>
     <row r="2" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="186" t="s">
+      <c r="A2" s="153" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="187"/>
-      <c r="C2" s="187"/>
-      <c r="D2" s="187"/>
-      <c r="E2" s="187"/>
-      <c r="F2" s="187"/>
-      <c r="G2" s="187"/>
-      <c r="H2" s="188"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="155"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="195" t="s">
+      <c r="A3" s="156" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="196"/>
-      <c r="C3" s="196"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="195" t="s">
+      <c r="B3" s="157"/>
+      <c r="C3" s="157"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="197"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="157"/>
+      <c r="H3" s="158"/>
     </row>
     <row r="4" spans="1:11" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="146" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="138" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="135" t="s">
         <v>52</v>
-      </c>
-      <c r="B5" s="135" t="s">
-        <v>53</v>
       </c>
       <c r="C5" s="125">
         <v>1</v>
@@ -4028,7 +4028,7 @@
       </c>
       <c r="E5" s="99"/>
       <c r="F5" s="125" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G5" s="125" t="s">
         <v>4</v>
@@ -4055,10 +4055,10 @@
         <v>3</v>
       </c>
       <c r="G6" s="125" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H6" s="119" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
@@ -4076,18 +4076,18 @@
       </c>
       <c r="E7" s="99"/>
       <c r="F7" s="125" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G7" s="125" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H7" s="122" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A8" s="138" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="135" t="s">
         <v>21</v>
@@ -4100,21 +4100,21 @@
       </c>
       <c r="E8" s="99"/>
       <c r="F8" s="124" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G8" s="124" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H8" s="122" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A9" s="138" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="135" t="s">
         <v>55</v>
-      </c>
-      <c r="B9" s="135" t="s">
-        <v>56</v>
       </c>
       <c r="C9" s="125">
         <v>3</v>
@@ -4124,13 +4124,13 @@
       </c>
       <c r="E9" s="101"/>
       <c r="F9" s="100" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G9" s="100" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H9" s="61" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -4159,10 +4159,10 @@
     </row>
     <row r="11" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="139" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="140" t="s">
         <v>57</v>
-      </c>
-      <c r="B11" s="140" t="s">
-        <v>58</v>
       </c>
       <c r="C11" s="129">
         <v>3</v>
@@ -4172,13 +4172,13 @@
       </c>
       <c r="E11" s="102"/>
       <c r="F11" s="114" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G11" s="114" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H11" s="118" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J11" s="116" t="s">
         <v>12</v>
@@ -4188,18 +4188,18 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="225" t="s">
+      <c r="A12" s="159" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="226"/>
+      <c r="B12" s="160"/>
       <c r="C12" s="4">
         <v>18</v>
       </c>
-      <c r="D12" s="164"/>
-      <c r="E12" s="160"/>
-      <c r="F12" s="160"/>
-      <c r="G12" s="160"/>
-      <c r="H12" s="160"/>
+      <c r="D12" s="161"/>
+      <c r="E12" s="162"/>
+      <c r="F12" s="162"/>
+      <c r="G12" s="162"/>
+      <c r="H12" s="162"/>
       <c r="J12" s="117" t="s">
         <v>29</v>
       </c>
@@ -4216,10 +4216,10 @@
     </row>
     <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="104" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B14" s="145" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C14" s="104">
         <v>3</v>
@@ -4227,12 +4227,12 @@
       <c r="D14" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="192" t="s">
-        <v>147</v>
-      </c>
-      <c r="F14" s="193"/>
-      <c r="G14" s="193"/>
-      <c r="H14" s="194"/>
+      <c r="E14" s="147" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14" s="148"/>
+      <c r="G14" s="148"/>
+      <c r="H14" s="149"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4254,7 +4254,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4263,75 +4263,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="165" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="167"/>
+      <c r="A1" s="150" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="152"/>
     </row>
     <row r="2" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="175" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="170"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="177"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="195" t="s">
+      <c r="A3" s="156" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="196"/>
-      <c r="C3" s="196"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="195" t="s">
+      <c r="B3" s="157"/>
+      <c r="C3" s="157"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="196"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="197"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="157"/>
+      <c r="H3" s="158"/>
     </row>
     <row r="4" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="146" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A5" s="136" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="137" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="130">
         <v>3</v>
@@ -4341,7 +4341,7 @@
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="132" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G5" s="132" t="s">
         <v>1</v>
@@ -4352,7 +4352,7 @@
     </row>
     <row r="6" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A6" s="138" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" s="135" t="s">
         <v>44</v>
@@ -4365,21 +4365,21 @@
       </c>
       <c r="E6" s="69"/>
       <c r="F6" s="133" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G6" s="133" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H6" s="98" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A7" s="138" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7" s="135" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C7" s="125">
         <v>3</v>
@@ -4389,18 +4389,18 @@
       </c>
       <c r="E7" s="113"/>
       <c r="F7" s="127" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G7" s="127" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H7" s="128" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A8" s="138" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8" s="135" t="s">
         <v>47</v>
@@ -4424,7 +4424,7 @@
     </row>
     <row r="9" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A9" s="138" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9" s="135" t="s">
         <v>15</v>
@@ -4437,36 +4437,36 @@
       </c>
       <c r="E9" s="69"/>
       <c r="F9" s="124" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G9" s="124" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H9" s="122" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="148" t="s">
-        <v>79</v>
+      <c r="A10" s="171" t="s">
+        <v>77</v>
       </c>
       <c r="B10" s="135" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="150">
+        <v>59</v>
+      </c>
+      <c r="C10" s="173">
         <v>3</v>
       </c>
-      <c r="D10" s="150" t="s">
+      <c r="D10" s="173" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="202"/>
-      <c r="F10" s="198" t="s">
+      <c r="E10" s="163"/>
+      <c r="F10" s="178" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="198" t="s">
+      <c r="G10" s="178" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="200" t="s">
+      <c r="H10" s="180" t="s">
         <v>2</v>
       </c>
       <c r="J10" s="115" t="s">
@@ -4477,16 +4477,16 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="158"/>
+      <c r="A11" s="172"/>
       <c r="B11" s="140" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="159"/>
-      <c r="D11" s="159"/>
-      <c r="E11" s="203"/>
-      <c r="F11" s="199"/>
-      <c r="G11" s="199"/>
-      <c r="H11" s="201"/>
+        <v>60</v>
+      </c>
+      <c r="C11" s="174"/>
+      <c r="D11" s="174"/>
+      <c r="E11" s="164"/>
+      <c r="F11" s="179"/>
+      <c r="G11" s="179"/>
+      <c r="H11" s="181"/>
       <c r="J11" s="116" t="s">
         <v>12</v>
       </c>
@@ -4495,10 +4495,10 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="156" t="s">
+      <c r="A12" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="157"/>
+      <c r="B12" s="166"/>
       <c r="C12" s="13">
         <v>16</v>
       </c>
@@ -4582,8 +4582,8 @@
       <c r="B18" s="72"/>
       <c r="C18" s="73"/>
       <c r="D18" s="73"/>
-      <c r="E18" s="222"/>
-      <c r="F18" s="223"/>
+      <c r="E18" s="167"/>
+      <c r="F18" s="168"/>
       <c r="G18" s="81"/>
       <c r="H18" s="41"/>
       <c r="I18" s="16"/>
@@ -4594,8 +4594,8 @@
       <c r="B19" s="39"/>
       <c r="C19" s="74"/>
       <c r="D19" s="74"/>
-      <c r="E19" s="220"/>
-      <c r="F19" s="221"/>
+      <c r="E19" s="169"/>
+      <c r="F19" s="170"/>
       <c r="G19" s="94"/>
       <c r="H19" s="41"/>
       <c r="I19" s="16"/>
@@ -4607,6 +4607,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="E18:F18"/>
@@ -4614,13 +4621,6 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4630,125 +4630,125 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="165" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="167"/>
+      <c r="A1" s="150" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="152"/>
       <c r="I1" s="16"/>
       <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="186" t="s">
+      <c r="A2" s="153" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="187"/>
-      <c r="C2" s="187"/>
-      <c r="D2" s="187"/>
-      <c r="E2" s="187"/>
-      <c r="F2" s="187"/>
-      <c r="G2" s="187"/>
-      <c r="H2" s="188"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="155"/>
       <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="188" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="190"/>
-      <c r="C3" s="190"/>
-      <c r="D3" s="191"/>
-      <c r="E3" s="189" t="s">
+      <c r="B3" s="189"/>
+      <c r="C3" s="189"/>
+      <c r="D3" s="190"/>
+      <c r="E3" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="190"/>
-      <c r="G3" s="190"/>
-      <c r="H3" s="191"/>
+      <c r="F3" s="189"/>
+      <c r="G3" s="189"/>
+      <c r="H3" s="190"/>
     </row>
     <row r="4" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="146" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A5" s="125" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" s="141" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" s="125">
         <v>2</v>
       </c>
       <c r="D5" s="125" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E5" s="126"/>
       <c r="F5" s="131" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G5" s="131" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H5" s="131" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A6" s="125" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" s="141" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" s="125">
         <v>1</v>
       </c>
       <c r="D6" s="125" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E6" s="126"/>
       <c r="F6" s="133" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G6" s="133" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H6" s="133" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
@@ -4766,13 +4766,13 @@
       </c>
       <c r="E7" s="126"/>
       <c r="F7" s="131" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G7" s="131" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H7" s="131" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
@@ -4790,21 +4790,21 @@
       </c>
       <c r="E8" s="126"/>
       <c r="F8" s="124" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G8" s="131" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H8" s="131" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A9" s="125" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B9" s="141" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9" s="125">
         <v>3</v>
@@ -4814,86 +4814,86 @@
       </c>
       <c r="E9" s="126"/>
       <c r="F9" s="124" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G9" s="124" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H9" s="124" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="150" t="s">
+      <c r="A10" s="173" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="141" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="173">
+        <v>3</v>
+      </c>
+      <c r="D10" s="173" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="192"/>
+      <c r="F10" s="193" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10" s="193" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" s="193" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="173"/>
+      <c r="B11" s="141" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="141" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="150">
+      <c r="C11" s="173"/>
+      <c r="D11" s="173"/>
+      <c r="E11" s="192"/>
+      <c r="F11" s="193"/>
+      <c r="G11" s="193"/>
+      <c r="H11" s="193"/>
+    </row>
+    <row r="12" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="173" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="141" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="173">
         <v>3</v>
       </c>
-      <c r="D10" s="150" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="151"/>
-      <c r="F10" s="181" t="s">
-        <v>132</v>
-      </c>
-      <c r="G10" s="181" t="s">
-        <v>132</v>
-      </c>
-      <c r="H10" s="181" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="150"/>
-      <c r="B11" s="141" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="150"/>
-      <c r="D11" s="150"/>
-      <c r="E11" s="151"/>
-      <c r="F11" s="181"/>
-      <c r="G11" s="181"/>
-      <c r="H11" s="181"/>
-    </row>
-    <row r="12" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="150" t="s">
+      <c r="D12" s="173" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="141" t="s">
+      <c r="E12" s="192"/>
+      <c r="F12" s="191" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="191" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="191" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="173"/>
+      <c r="B13" s="141" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="150">
-        <v>3</v>
-      </c>
-      <c r="D12" s="150" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="151"/>
-      <c r="F12" s="185" t="s">
-        <v>123</v>
-      </c>
-      <c r="G12" s="185" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="185" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="150"/>
-      <c r="B13" s="141" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="150"/>
-      <c r="D13" s="150"/>
-      <c r="E13" s="151"/>
-      <c r="F13" s="185"/>
-      <c r="G13" s="185"/>
-      <c r="H13" s="185"/>
+      <c r="C13" s="173"/>
+      <c r="D13" s="173"/>
+      <c r="E13" s="192"/>
+      <c r="F13" s="191"/>
+      <c r="G13" s="191"/>
+      <c r="H13" s="191"/>
       <c r="J13" s="115" t="s">
         <v>28</v>
       </c>
@@ -4903,18 +4903,18 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="156" t="s">
+      <c r="A14" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="157"/>
+      <c r="B14" s="166"/>
       <c r="C14" s="13">
         <v>16</v>
       </c>
-      <c r="D14" s="227"/>
-      <c r="E14" s="228"/>
-      <c r="F14" s="228"/>
-      <c r="G14" s="228"/>
-      <c r="H14" s="228"/>
+      <c r="D14" s="182"/>
+      <c r="E14" s="183"/>
+      <c r="F14" s="183"/>
+      <c r="G14" s="183"/>
+      <c r="H14" s="183"/>
       <c r="J14" s="116" t="s">
         <v>12</v>
       </c>
@@ -4956,53 +4956,46 @@
     </row>
     <row r="17" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A17" s="142" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B17" s="137" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C17" s="130">
         <v>3</v>
       </c>
       <c r="D17" s="121" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E17" s="110"/>
-      <c r="F17" s="177" t="s">
-        <v>142</v>
-      </c>
-      <c r="G17" s="177"/>
-      <c r="H17" s="146"/>
+      <c r="F17" s="184" t="s">
+        <v>140</v>
+      </c>
+      <c r="G17" s="184"/>
+      <c r="H17" s="185"/>
     </row>
     <row r="18" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="143" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B18" s="140" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C18" s="129">
         <v>1</v>
       </c>
       <c r="D18" s="114" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E18" s="68"/>
-      <c r="F18" s="178" t="s">
-        <v>142</v>
-      </c>
-      <c r="G18" s="178"/>
-      <c r="H18" s="179"/>
+      <c r="F18" s="186" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" s="186"/>
+      <c r="H18" s="187"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="A12:A13"/>
@@ -5018,6 +5011,13 @@
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5027,8 +5027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5037,112 +5037,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="165" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="167"/>
+      <c r="A1" s="150" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="152"/>
     </row>
     <row r="2" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="175" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="170"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="177"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="174" t="s">
+      <c r="A3" s="209" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="174" t="s">
+      <c r="B3" s="210"/>
+      <c r="C3" s="210"/>
+      <c r="D3" s="211"/>
+      <c r="E3" s="209" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="175"/>
-      <c r="G3" s="175"/>
-      <c r="H3" s="176"/>
+      <c r="F3" s="210"/>
+      <c r="G3" s="210"/>
+      <c r="H3" s="211"/>
     </row>
     <row r="4" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="146" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>161</v>
-      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="171" t="s">
+      <c r="A5" s="206" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="172" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="173">
+      <c r="B5" s="207" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="208">
         <v>3</v>
       </c>
-      <c r="D5" s="173" t="s">
+      <c r="D5" s="208" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="203"/>
+      <c r="F5" s="212" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="201" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="185" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="184"/>
-      <c r="F5" s="180" t="s">
-        <v>124</v>
-      </c>
-      <c r="G5" s="182" t="s">
-        <v>121</v>
-      </c>
-      <c r="H5" s="146" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="148"/>
-      <c r="B6" s="149"/>
-      <c r="C6" s="150"/>
-      <c r="D6" s="150"/>
-      <c r="E6" s="151"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="183"/>
-      <c r="H6" s="147"/>
+      <c r="A6" s="171"/>
+      <c r="B6" s="198"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="192"/>
+      <c r="F6" s="193"/>
+      <c r="G6" s="202"/>
+      <c r="H6" s="197"/>
     </row>
     <row r="7" spans="1:11" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="148"/>
-      <c r="B7" s="149"/>
-      <c r="C7" s="150"/>
-      <c r="D7" s="150"/>
-      <c r="E7" s="151"/>
-      <c r="F7" s="181"/>
-      <c r="G7" s="183"/>
-      <c r="H7" s="147"/>
+      <c r="A7" s="171"/>
+      <c r="B7" s="198"/>
+      <c r="C7" s="173"/>
+      <c r="D7" s="173"/>
+      <c r="E7" s="192"/>
+      <c r="F7" s="193"/>
+      <c r="G7" s="202"/>
+      <c r="H7" s="197"/>
     </row>
     <row r="8" spans="1:11" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="138" t="s">
@@ -5159,152 +5159,152 @@
       </c>
       <c r="E8" s="126"/>
       <c r="F8" s="133" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G8" s="133" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H8" s="98" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="148" t="s">
+      <c r="A9" s="171" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="198" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="173">
+        <v>3</v>
+      </c>
+      <c r="D9" s="173" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="192"/>
+      <c r="F9" s="194" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="194" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" s="195" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="171"/>
+      <c r="B10" s="198"/>
+      <c r="C10" s="173"/>
+      <c r="D10" s="173"/>
+      <c r="E10" s="192"/>
+      <c r="F10" s="194"/>
+      <c r="G10" s="194"/>
+      <c r="H10" s="195"/>
+    </row>
+    <row r="11" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="171" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="141" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="173">
+        <v>2</v>
+      </c>
+      <c r="D11" s="173" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="192"/>
+      <c r="F11" s="194" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" s="194" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" s="195" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="171"/>
+      <c r="B12" s="141" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="173"/>
+      <c r="D12" s="173"/>
+      <c r="E12" s="192"/>
+      <c r="F12" s="194"/>
+      <c r="G12" s="194"/>
+      <c r="H12" s="195"/>
+    </row>
+    <row r="13" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="171" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="141" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="149" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="150">
+      <c r="C13" s="173">
+        <v>1</v>
+      </c>
+      <c r="D13" s="173" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="192"/>
+      <c r="F13" s="194" t="s">
+        <v>153</v>
+      </c>
+      <c r="G13" s="196"/>
+      <c r="H13" s="200"/>
+    </row>
+    <row r="14" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="171"/>
+      <c r="B14" s="141" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="173"/>
+      <c r="D14" s="173"/>
+      <c r="E14" s="192"/>
+      <c r="F14" s="194"/>
+      <c r="G14" s="196"/>
+      <c r="H14" s="200"/>
+    </row>
+    <row r="15" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="171" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="141" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="173">
         <v>3</v>
       </c>
-      <c r="D9" s="150" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="151"/>
-      <c r="F9" s="152" t="s">
-        <v>130</v>
-      </c>
-      <c r="G9" s="152" t="s">
-        <v>130</v>
-      </c>
-      <c r="H9" s="153" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="148"/>
-      <c r="B10" s="149"/>
-      <c r="C10" s="150"/>
-      <c r="D10" s="150"/>
-      <c r="E10" s="151"/>
-      <c r="F10" s="152"/>
-      <c r="G10" s="152"/>
-      <c r="H10" s="153"/>
-    </row>
-    <row r="11" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="148" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="141" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="150">
-        <v>2</v>
-      </c>
-      <c r="D11" s="150" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="151"/>
-      <c r="F11" s="152" t="s">
-        <v>155</v>
-      </c>
-      <c r="G11" s="152" t="s">
-        <v>155</v>
-      </c>
-      <c r="H11" s="153" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="148"/>
-      <c r="B12" s="141" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="150"/>
-      <c r="D12" s="150"/>
-      <c r="E12" s="151"/>
-      <c r="F12" s="152"/>
-      <c r="G12" s="152"/>
-      <c r="H12" s="153"/>
-    </row>
-    <row r="13" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="148" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="141" t="s">
+      <c r="D15" s="173" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="192"/>
+      <c r="F15" s="194" t="s">
+        <v>127</v>
+      </c>
+      <c r="G15" s="194" t="s">
+        <v>127</v>
+      </c>
+      <c r="H15" s="195" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="172"/>
+      <c r="B16" s="144" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="150">
-        <v>1</v>
-      </c>
-      <c r="D13" s="150" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="151"/>
-      <c r="F13" s="152" t="s">
-        <v>155</v>
-      </c>
-      <c r="G13" s="155"/>
-      <c r="H13" s="154"/>
-    </row>
-    <row r="14" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="148"/>
-      <c r="B14" s="141" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="150"/>
-      <c r="D14" s="150"/>
-      <c r="E14" s="151"/>
-      <c r="F14" s="152"/>
-      <c r="G14" s="155"/>
-      <c r="H14" s="154"/>
-    </row>
-    <row r="15" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="148" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" s="141" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="150">
-        <v>3</v>
-      </c>
-      <c r="D15" s="150" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="151"/>
-      <c r="F15" s="152" t="s">
-        <v>129</v>
-      </c>
-      <c r="G15" s="152" t="s">
-        <v>129</v>
-      </c>
-      <c r="H15" s="153" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="158"/>
-      <c r="B16" s="144" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="163"/>
-      <c r="F16" s="161"/>
-      <c r="G16" s="161"/>
-      <c r="H16" s="162"/>
+      <c r="C16" s="174"/>
+      <c r="D16" s="174"/>
+      <c r="E16" s="199"/>
+      <c r="F16" s="204"/>
+      <c r="G16" s="204"/>
+      <c r="H16" s="205"/>
       <c r="J16" s="115" t="s">
         <v>28</v>
       </c>
@@ -5313,18 +5313,18 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="156" t="s">
+      <c r="A17" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="157"/>
+      <c r="B17" s="166"/>
       <c r="C17" s="13">
         <v>15</v>
       </c>
-      <c r="D17" s="160"/>
-      <c r="E17" s="160"/>
-      <c r="F17" s="160"/>
-      <c r="G17" s="160"/>
-      <c r="H17" s="160"/>
+      <c r="D17" s="162"/>
+      <c r="E17" s="162"/>
+      <c r="F17" s="162"/>
+      <c r="G17" s="162"/>
+      <c r="H17" s="162"/>
       <c r="J17" s="116" t="s">
         <v>12</v>
       </c>
@@ -5348,11 +5348,31 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:H17"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="H13:H14"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="C13:C14"/>
@@ -5362,35 +5382,15 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="H13:H14"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="E5:E7"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:H17"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:H10">
@@ -5420,29 +5420,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="165" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="167"/>
+      <c r="A1" s="150" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="152"/>
     </row>
     <row r="2" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="217"/>
-      <c r="B2" s="218"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="219"/>
+      <c r="A2" s="224"/>
+      <c r="B2" s="225"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="226"/>
     </row>
     <row r="3" spans="1:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="175" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="170"/>
+      <c r="B3" s="176"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="177"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -5470,7 +5470,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="45"/>
       <c r="B5" s="53" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C5" s="110">
         <v>1</v>
@@ -5485,7 +5485,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="46"/>
       <c r="B6" s="25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" s="107">
         <v>2</v>
@@ -5500,7 +5500,7 @@
     <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="52"/>
       <c r="B7" s="24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" s="107">
         <v>2</v>
@@ -5513,7 +5513,7 @@
     <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="52"/>
       <c r="B8" s="24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" s="107">
         <v>3</v>
@@ -5526,7 +5526,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
       <c r="B9" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C9" s="107">
         <v>3</v>
@@ -5537,7 +5537,7 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="52"/>
       <c r="B10" s="24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C10" s="107">
         <v>2</v>
@@ -5548,7 +5548,7 @@
     <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="52"/>
       <c r="B11" s="24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C11" s="107">
         <v>3</v>
@@ -5598,10 +5598,10 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="204" t="s">
+      <c r="A15" s="227" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="205"/>
+      <c r="B15" s="228"/>
       <c r="C15" s="4">
         <f>SUM(C5:C14)</f>
         <v>16</v>
@@ -5616,29 +5616,29 @@
     </row>
     <row r="16" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="206" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17" s="207"/>
-      <c r="C17" s="207"/>
-      <c r="D17" s="207"/>
-      <c r="E17" s="208"/>
+      <c r="A17" s="213" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="214"/>
+      <c r="C17" s="214"/>
+      <c r="D17" s="214"/>
+      <c r="E17" s="215"/>
     </row>
     <row r="18" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="209"/>
-      <c r="B18" s="210"/>
-      <c r="C18" s="210"/>
-      <c r="D18" s="210"/>
-      <c r="E18" s="211"/>
+      <c r="A18" s="216"/>
+      <c r="B18" s="217"/>
+      <c r="C18" s="217"/>
+      <c r="D18" s="217"/>
+      <c r="E18" s="218"/>
     </row>
     <row r="19" spans="1:8" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="212" t="s">
+      <c r="A19" s="219" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="213"/>
-      <c r="C19" s="213"/>
-      <c r="D19" s="213"/>
-      <c r="E19" s="214"/>
+      <c r="B19" s="220"/>
+      <c r="C19" s="220"/>
+      <c r="D19" s="220"/>
+      <c r="E19" s="221"/>
     </row>
     <row r="20" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="58" t="s">
@@ -5660,7 +5660,7 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="51"/>
       <c r="B21" s="44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C21" s="27">
         <v>2</v>
@@ -5671,7 +5671,7 @@
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="52"/>
       <c r="B22" s="32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C22" s="97">
         <v>1</v>
@@ -5682,7 +5682,7 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
       <c r="B23" s="31" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C23" s="97">
         <v>2</v>
@@ -5693,7 +5693,7 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
       <c r="B24" s="78" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C24" s="79">
         <v>1</v>
@@ -5704,7 +5704,7 @@
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
       <c r="B25" s="78" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C25" s="79">
         <v>2</v>
@@ -5715,7 +5715,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="28"/>
       <c r="B26" s="78" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C26" s="79">
         <v>1</v>
@@ -5726,7 +5726,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="28"/>
       <c r="B27" s="78" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C27" s="79">
         <v>2</v>
@@ -5737,7 +5737,7 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="28"/>
       <c r="B28" s="78" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C28" s="79">
         <v>1</v>
@@ -5748,7 +5748,7 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
       <c r="B29" s="82" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C29" s="106">
         <v>2</v>
@@ -5759,7 +5759,7 @@
     <row r="30" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="28"/>
       <c r="B30" s="31" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C30" s="97">
         <v>1</v>
@@ -5804,10 +5804,10 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="215" t="s">
+      <c r="A33" s="222" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="216"/>
+      <c r="B33" s="223"/>
       <c r="C33" s="14">
         <f>SUM(C21:C32)</f>
         <v>18</v>
@@ -5822,29 +5822,29 @@
     </row>
     <row r="34" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="206" t="s">
-        <v>117</v>
-      </c>
-      <c r="B35" s="207"/>
-      <c r="C35" s="207"/>
-      <c r="D35" s="207"/>
-      <c r="E35" s="208"/>
+      <c r="A35" s="213" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="214"/>
+      <c r="C35" s="214"/>
+      <c r="D35" s="214"/>
+      <c r="E35" s="215"/>
     </row>
     <row r="36" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="209"/>
-      <c r="B36" s="210"/>
-      <c r="C36" s="210"/>
-      <c r="D36" s="210"/>
-      <c r="E36" s="211"/>
+      <c r="A36" s="216"/>
+      <c r="B36" s="217"/>
+      <c r="C36" s="217"/>
+      <c r="D36" s="217"/>
+      <c r="E36" s="218"/>
     </row>
     <row r="37" spans="1:8" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="212" t="s">
+      <c r="A37" s="219" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="213"/>
-      <c r="C37" s="213"/>
-      <c r="D37" s="213"/>
-      <c r="E37" s="214"/>
+      <c r="B37" s="220"/>
+      <c r="C37" s="220"/>
+      <c r="D37" s="220"/>
+      <c r="E37" s="221"/>
     </row>
     <row r="38" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="109" t="s">
@@ -5866,7 +5866,7 @@
     <row r="39" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A39" s="51"/>
       <c r="B39" s="112" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C39" s="27">
         <v>3</v>
@@ -5877,7 +5877,7 @@
     <row r="40" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A40" s="52"/>
       <c r="B40" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C40" s="97">
         <v>1</v>
@@ -5888,7 +5888,7 @@
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="28"/>
       <c r="B41" s="78" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C41" s="97">
         <v>3</v>
@@ -5899,7 +5899,7 @@
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="28"/>
       <c r="B42" s="78" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C42" s="79">
         <v>1</v>
@@ -5910,7 +5910,7 @@
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="28"/>
       <c r="B43" s="78" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C43" s="79">
         <v>3</v>
@@ -5921,7 +5921,7 @@
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="28"/>
       <c r="B44" s="78" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C44" s="79">
         <v>1</v>
@@ -5932,7 +5932,7 @@
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="28"/>
       <c r="B45" s="82" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C45" s="79">
         <v>2</v>
@@ -5943,7 +5943,7 @@
     <row r="46" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A46" s="28"/>
       <c r="B46" s="111" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C46" s="79">
         <v>3</v>
@@ -5954,7 +5954,7 @@
     <row r="47" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="28"/>
       <c r="B47" s="111" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C47" s="106">
         <v>1</v>
@@ -6002,10 +6002,10 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="215" t="s">
+      <c r="A51" s="222" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="216"/>
+      <c r="B51" s="223"/>
       <c r="C51" s="14">
         <f>SUM(C39:C50)</f>
         <v>18</v>

</xml_diff>

<commit_message>
FYP Evaluation Finalization I
Changing the Backend Implementation for DB OneEyeOwl
</commit_message>
<xml_diff>
--- a/Templates/Allocation and Offering Tester.xlsx
+++ b/Templates/Allocation and Offering Tester.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" tabRatio="756"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" tabRatio="756" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BCSE-3 (Spring-2016 Batch)" sheetId="14" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="100">
   <si>
     <t>Dr. Arif Jamal</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Ethics</t>
   </si>
   <si>
-    <t>(University Elective – II)</t>
-  </si>
-  <si>
     <t>SEN 311</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>Formal Methods in Software Engineering</t>
   </si>
   <si>
-    <t>(SE Supporting –I)</t>
-  </si>
-  <si>
     <t>CSC 2031</t>
   </si>
   <si>
@@ -218,9 +212,6 @@
   </si>
   <si>
     <t>CSC 351</t>
-  </si>
-  <si>
-    <t>(SE Elective –I)</t>
   </si>
   <si>
     <t>Discrete Structures</t>
@@ -474,7 +465,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -832,6 +823,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="443">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1278,7 +1308,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1533,6 +1563,33 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1563,32 +1620,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1617,14 +1656,14 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="443">
@@ -3334,8 +3373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3347,7 +3386,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" s="74"/>
@@ -3359,7 +3398,7 @@
     </row>
     <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="76" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B2" s="77"/>
       <c r="C2" s="77"/>
@@ -3391,22 +3430,22 @@
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -3424,7 +3463,7 @@
       </c>
       <c r="E5" s="33"/>
       <c r="F5" s="49" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G5" s="49" t="s">
         <v>4</v>
@@ -3451,10 +3490,10 @@
         <v>3</v>
       </c>
       <c r="G6" s="49" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H6" s="44" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -3472,13 +3511,13 @@
       </c>
       <c r="E7" s="33"/>
       <c r="F7" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="47" t="s">
         <v>79</v>
-      </c>
-      <c r="G7" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" s="47" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -3496,13 +3535,13 @@
       </c>
       <c r="E8" s="33"/>
       <c r="F8" s="48" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G8" s="48" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H8" s="47" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -3520,13 +3559,13 @@
       </c>
       <c r="E9" s="35"/>
       <c r="F9" s="34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3562,13 +3601,13 @@
       </c>
       <c r="E11" s="36"/>
       <c r="F11" s="42" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H11" s="43" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3590,10 +3629,10 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B14" s="68" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C14" s="38">
         <v>3</v>
@@ -3602,7 +3641,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="70" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F14" s="71"/>
       <c r="G14" s="71"/>
@@ -3628,7 +3667,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3638,7 +3677,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="73" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" s="74"/>
@@ -3649,16 +3688,16 @@
       <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="98"/>
+      <c r="A2" s="86" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="88"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="79" t="s">
@@ -3682,27 +3721,27 @@
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" s="61" t="s">
         <v>38</v>
@@ -3715,7 +3754,7 @@
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="56" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G5" s="56" t="s">
         <v>1</v>
@@ -3726,7 +3765,7 @@
     </row>
     <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" s="59" t="s">
         <v>29</v>
@@ -3739,21 +3778,21 @@
       </c>
       <c r="E6" s="23"/>
       <c r="F6" s="57" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G6" s="57" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="59" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C7" s="49">
         <v>3</v>
@@ -3763,18 +3802,18 @@
       </c>
       <c r="E7" s="41"/>
       <c r="F7" s="51" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G7" s="51" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H7" s="52" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" s="59" t="s">
         <v>30</v>
@@ -3798,7 +3837,7 @@
     </row>
     <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" s="59" t="s">
         <v>11</v>
@@ -3811,56 +3850,54 @@
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="48" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G9" s="48" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H9" s="47" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="92" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="59" t="s">
+      <c r="A10" s="101" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="94">
+      <c r="C10" s="103">
         <v>3</v>
       </c>
-      <c r="D10" s="94" t="s">
+      <c r="D10" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="103"/>
-      <c r="F10" s="99" t="s">
+      <c r="E10" s="93"/>
+      <c r="F10" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="99" t="s">
+      <c r="G10" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="101" t="s">
+      <c r="H10" s="91" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="93"/>
-      <c r="B11" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="104"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="100"/>
-      <c r="H11" s="102"/>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="102"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="92"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="86" t="s">
+      <c r="A12" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="87"/>
+      <c r="B12" s="96"/>
       <c r="C12" s="4">
         <v>16</v>
       </c>
@@ -3927,8 +3964,8 @@
       <c r="B18" s="24"/>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="89"/>
+      <c r="E18" s="97"/>
+      <c r="F18" s="98"/>
       <c r="G18" s="27"/>
       <c r="H18" s="16"/>
     </row>
@@ -3937,13 +3974,20 @@
       <c r="B19" s="14"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
-      <c r="E19" s="90"/>
-      <c r="F19" s="91"/>
+      <c r="E19" s="99"/>
+      <c r="F19" s="100"/>
       <c r="G19" s="31"/>
       <c r="H19" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B10:B11"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:D3"/>
@@ -3952,12 +3996,6 @@
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3967,15 +4005,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" s="74"/>
@@ -3987,7 +4025,7 @@
     </row>
     <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="76" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B2" s="77"/>
       <c r="C2" s="77"/>
@@ -3998,18 +4036,18 @@
       <c r="H2" s="78"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="111" t="s">
+      <c r="B3" s="115"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="113"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="116"/>
     </row>
     <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
@@ -4019,70 +4057,70 @@
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="65" t="s">
         <v>41</v>
-      </c>
-      <c r="B5" s="65" t="s">
-        <v>42</v>
       </c>
       <c r="C5" s="49">
         <v>2</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="50"/>
       <c r="F5" s="55" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G5" s="55" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H5" s="55" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="65" t="s">
         <v>44</v>
-      </c>
-      <c r="B6" s="65" t="s">
-        <v>45</v>
       </c>
       <c r="C6" s="49">
         <v>1</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="50"/>
       <c r="F6" s="57" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G6" s="57" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H6" s="57" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -4100,13 +4138,13 @@
       </c>
       <c r="E7" s="50"/>
       <c r="F7" s="55" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G7" s="55" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H7" s="55" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -4124,21 +4162,21 @@
       </c>
       <c r="E8" s="50"/>
       <c r="F8" s="48" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G8" s="55" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H8" s="55" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="65" t="s">
         <v>46</v>
-      </c>
-      <c r="B9" s="65" t="s">
-        <v>47</v>
       </c>
       <c r="C9" s="49">
         <v>3</v>
@@ -4148,100 +4186,96 @@
       </c>
       <c r="E9" s="50"/>
       <c r="F9" s="48" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G9" s="48" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H9" s="48" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="94" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="117" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="65" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="94">
+      <c r="C10" s="103">
         <v>3</v>
       </c>
-      <c r="D10" s="94" t="s">
+      <c r="D10" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="115"/>
-      <c r="F10" s="116" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" s="116" t="s">
-        <v>69</v>
-      </c>
-      <c r="H10" s="116" t="s">
-        <v>69</v>
+      <c r="E10" s="106"/>
+      <c r="F10" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="107" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="94"/>
-      <c r="B11" s="65" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="94"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="116"/>
-      <c r="G11" s="116"/>
-      <c r="H11" s="116"/>
-    </row>
-    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="94" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="65" t="s">
+      <c r="A11" s="103"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="107"/>
+      <c r="G11" s="107"/>
+      <c r="H11" s="107"/>
+    </row>
+    <row r="12" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="103" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="117" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="103">
+        <v>3</v>
+      </c>
+      <c r="D12" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="94">
-        <v>3</v>
-      </c>
-      <c r="D12" s="94" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="115"/>
-      <c r="F12" s="114" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="114" t="s">
+      <c r="E12" s="106"/>
+      <c r="F12" s="105" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="114" t="s">
+      <c r="H12" s="105" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="94"/>
-      <c r="B13" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="94"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="114"/>
-      <c r="G13" s="114"/>
-      <c r="H13" s="114"/>
+      <c r="A13" s="103"/>
+      <c r="B13" s="119"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="106"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="105"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="86" t="s">
+      <c r="A14" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="87"/>
+      <c r="B14" s="96"/>
       <c r="C14" s="4">
         <v>16</v>
       </c>
-      <c r="D14" s="105"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="106"/>
-      <c r="G14" s="106"/>
-      <c r="H14" s="106"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="109"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="109"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -4267,46 +4301,55 @@
     </row>
     <row r="17" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A17" s="66" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B17" s="61" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C17" s="54">
         <v>3</v>
       </c>
       <c r="D17" s="46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E17" s="40"/>
-      <c r="F17" s="107" t="s">
-        <v>79</v>
-      </c>
-      <c r="G17" s="107"/>
-      <c r="H17" s="108"/>
+      <c r="F17" s="110" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="110"/>
+      <c r="H17" s="111"/>
     </row>
     <row r="18" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="67" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B18" s="64" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C18" s="53">
         <v>1</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E18" s="22"/>
-      <c r="F18" s="109" t="s">
-        <v>79</v>
-      </c>
-      <c r="G18" s="109"/>
-      <c r="H18" s="110"/>
+      <c r="F18" s="112" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="112"/>
+      <c r="H18" s="113"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="24">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="A12:A13"/>
@@ -4322,13 +4365,6 @@
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>